<commit_message>
Fixed Chapter 1-4 and 6-7
- Fixed phonemes to syllables
- Updates references
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabagita Ivan\Desktop\Skripsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C940EDE-3C6E-4A32-9312-24F8DE0356F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC983136-3BFC-4872-9ADD-03BBD2669C4E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="2" activeTab="7" xr2:uid="{8639E025-6890-4D88-A143-6E789D4DC52A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{8639E025-6890-4D88-A143-6E789D4DC52A}"/>
   </bookViews>
   <sheets>
     <sheet name="3.1" sheetId="6" r:id="rId1"/>
@@ -27,6 +27,12 @@
     <sheet name="4.3" sheetId="3" r:id="rId12"/>
     <sheet name="4.4" sheetId="4" r:id="rId13"/>
     <sheet name="4.5" sheetId="5" r:id="rId14"/>
+    <sheet name="6.1" sheetId="15" r:id="rId15"/>
+    <sheet name="6.2" sheetId="16" r:id="rId16"/>
+    <sheet name="6.3" sheetId="17" r:id="rId17"/>
+    <sheet name="6.4" sheetId="18" r:id="rId18"/>
+    <sheet name="6.5" sheetId="19" r:id="rId19"/>
+    <sheet name="6.6" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="166">
   <si>
     <t>No</t>
   </si>
@@ -175,9 +181,6 @@
     <t>Click Start button.</t>
   </si>
   <si>
-    <t>Phonemes page is shown.</t>
-  </si>
-  <si>
     <t>Alternate Course</t>
   </si>
   <si>
@@ -199,27 +202,15 @@
     <t>UC02</t>
   </si>
   <si>
-    <t>This use-case describes the event when user opens Phonemes page.</t>
-  </si>
-  <si>
     <t>User clicks Start button from Home page.</t>
   </si>
   <si>
-    <t>User opens Phonemes page.</t>
-  </si>
-  <si>
-    <t>Click Record button and say asked phoneme.</t>
-  </si>
-  <si>
     <t>Record the speech and upload to save it.</t>
   </si>
   <si>
     <t>Click Next button.</t>
   </si>
   <si>
-    <t>Next Phonemes or Home page is shown.</t>
-  </si>
-  <si>
     <t>Recorded speech is played on audio element.</t>
   </si>
   <si>
@@ -335,6 +326,222 @@
   </si>
   <si>
     <t>Convert data to model's input and output.</t>
+  </si>
+  <si>
+    <t>Syllables page is shown.</t>
+  </si>
+  <si>
+    <t>This use-case describes the event when user opens Syllables page.</t>
+  </si>
+  <si>
+    <t>User opens Syllables page.</t>
+  </si>
+  <si>
+    <t>Next Syllables or Home page is shown.</t>
+  </si>
+  <si>
+    <t>Click Record button and say asked syllable.</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Access Home page</t>
+  </si>
+  <si>
+    <t>Home page is shown</t>
+  </si>
+  <si>
+    <t>As expected</t>
+  </si>
+  <si>
+    <t>Access Syllables page</t>
+  </si>
+  <si>
+    <t>Syllables page is shown</t>
+  </si>
+  <si>
+    <t>Process upload record request</t>
+  </si>
+  <si>
+    <t>Printed process results information on the console</t>
+  </si>
+  <si>
+    <t>Direct to Syllables page</t>
+  </si>
+  <si>
+    <t>Directed to Syllables page</t>
+  </si>
+  <si>
+    <t>Direct to Mimic application Home page</t>
+  </si>
+  <si>
+    <t>Directed to Mimic application Home page</t>
+  </si>
+  <si>
+    <t>Upload the record</t>
+  </si>
+  <si>
+    <t>Audio element is shown with the user record</t>
+  </si>
+  <si>
+    <t>Direct to the next Syllables page or direct back to Home page</t>
+  </si>
+  <si>
+    <t>Directed to the next Syllables page or Directed back to Home Page</t>
+  </si>
+  <si>
+    <t>Load and split collected data</t>
+  </si>
+  <si>
+    <t>Printed information on the console</t>
+  </si>
+  <si>
+    <t>Extract the data</t>
+  </si>
+  <si>
+    <t>Get corresponding batch data</t>
+  </si>
+  <si>
+    <t>Train the TensorFlow model to fit batch train data</t>
+  </si>
+  <si>
+    <t>Test the TensorFlow model from test data</t>
+  </si>
+  <si>
+    <t>Save the TensorFlow model to database</t>
+  </si>
+  <si>
+    <t>Recorded document in mimic_speech database models collection</t>
+  </si>
+  <si>
+    <t>Access Identify page</t>
+  </si>
+  <si>
+    <t>Identify page is shown</t>
+  </si>
+  <si>
+    <t>Access Generate page</t>
+  </si>
+  <si>
+    <t>Generate page is shown</t>
+  </si>
+  <si>
+    <t>Process upload record on Identify request</t>
+  </si>
+  <si>
+    <t>Process identify speech on Identify request</t>
+  </si>
+  <si>
+    <t>Process load speech data on Generate request</t>
+  </si>
+  <si>
+    <t>Process generate speech on Generate request</t>
+  </si>
+  <si>
+    <t>Direct to Identify page</t>
+  </si>
+  <si>
+    <t>Directed to Identify page</t>
+  </si>
+  <si>
+    <t>Direct to Generate page</t>
+  </si>
+  <si>
+    <t>Directed to Generate page</t>
+  </si>
+  <si>
+    <t>Direct to Collect application Home page</t>
+  </si>
+  <si>
+    <t>Directed to Collect application Home page</t>
+  </si>
+  <si>
+    <t>Send form for identify speech</t>
+  </si>
+  <si>
+    <t>Alert information despite success or error in the process</t>
+  </si>
+  <si>
+    <t>Direct back to Home page from Identify page</t>
+  </si>
+  <si>
+    <t>Directed back to Home Page</t>
+  </si>
+  <si>
+    <t>Load speech data</t>
+  </si>
+  <si>
+    <t>Datalist element store the speech data or alert if no speech data is found</t>
+  </si>
+  <si>
+    <t>Send form for generate speech</t>
+  </si>
+  <si>
+    <t>Audio element is shown with the generated speech or alert if error is occurred</t>
+  </si>
+  <si>
+    <t>Direct back to Home page from Generate page</t>
+  </si>
+  <si>
+    <t>Syllable</t>
+  </si>
+  <si>
+    <t>Noisy Background</t>
+  </si>
+  <si>
+    <t>Semi Noisy Background</t>
+  </si>
+  <si>
+    <t>No Noisy Background</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>/3</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>ma</t>
+  </si>
+  <si>
+    <t>mu</t>
+  </si>
+  <si>
+    <t>di</t>
+  </si>
+  <si>
+    <t>ri</t>
+  </si>
+  <si>
+    <t>ku</t>
+  </si>
+  <si>
+    <t>kan</t>
+  </si>
+  <si>
+    <t>Unknown 1</t>
+  </si>
+  <si>
+    <t>Unknown 2</t>
+  </si>
+  <si>
+    <t>Unknown 3</t>
   </si>
 </sst>
 </file>
@@ -489,13 +696,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -507,13 +714,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -835,12 +1042,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC4C3623-1849-4364-A121-3CC58B3A593B}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -882,6 +1090,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -939,6 +1148,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -995,6 +1205,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1061,6 +1272,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1143,6 +1355,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1200,6 +1413,968 @@
       </c>
       <c r="B7" s="4" t="s">
         <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED1886F-FB36-484B-9C90-633822D1B9B6}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C103172-6AE3-4850-B028-8EAC9886CE1D}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2665DF4-BB57-4BBC-912E-60371A920537}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5626A6E2-3CB9-4228-9242-32A8CDB5C5F8}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D33671-D8B4-4307-A64E-64BE16F5FD15}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1217,6 +2392,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1234,6 +2410,231 @@
       </c>
       <c r="B2" s="4" t="s">
         <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F672DFE2-C1D2-4C9E-9FCE-701CE27F0D30}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1251,6 +2652,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1296,7 +2698,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,13 +2712,13 @@
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="7"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1325,7 +2727,7 @@
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1334,7 +2736,7 @@
       <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1343,7 +2745,7 @@
       <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -1352,7 +2754,7 @@
       <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -1361,7 +2763,7 @@
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -1370,7 +2772,7 @@
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -1379,7 +2781,7 @@
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -1391,25 +2793,25 @@
       <c r="A10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>36</v>
@@ -1417,17 +2819,17 @@
       <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>36</v>
@@ -1435,8 +2837,8 @@
       <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>50</v>
+      <c r="A15" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>36</v>
@@ -1445,11 +2847,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -1459,6 +2856,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1469,7 +2871,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,22 +2885,22 @@
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>52</v>
-      </c>
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1507,7 +2909,7 @@
       <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1516,7 +2918,7 @@
       <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -1525,7 +2927,7 @@
       <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -1534,29 +2936,29 @@
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="C9" s="10"/>
     </row>
@@ -1564,54 +2966,54 @@
       <c r="A10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>57</v>
+      <c r="A11" s="12"/>
+      <c r="B11" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="B14" s="9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>49</v>
+      <c r="A15" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>36</v>
@@ -1619,8 +3021,8 @@
       <c r="C15" s="10"/>
     </row>
     <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>50</v>
+      <c r="A16" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>36</v>
@@ -1629,11 +3031,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B14:C14"/>
@@ -1643,6 +3040,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1667,22 +3069,22 @@
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="7"/>
+      <c r="B1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1691,7 +3093,7 @@
       <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1700,7 +3102,7 @@
       <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -1709,7 +3111,7 @@
       <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -1718,16 +3120,16 @@
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -1736,11 +3138,11 @@
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C9" s="10"/>
     </row>
@@ -1748,51 +3150,51 @@
       <c r="A10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14" t="s">
-        <v>65</v>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14" t="s">
-        <v>66</v>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14" t="s">
-        <v>98</v>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14" t="s">
-        <v>67</v>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14" t="s">
-        <v>68</v>
+      <c r="A15" s="12"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>46</v>
+      <c r="A16" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>36</v>
@@ -1800,26 +3202,26 @@
       <c r="C16" s="10"/>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>47</v>
+      <c r="A17" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C17" s="10"/>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="10"/>
-    </row>
-    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>36</v>
@@ -1828,11 +3230,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
@@ -1842,6 +3239,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1866,22 +3268,22 @@
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="7"/>
+      <c r="B1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1890,7 +3292,7 @@
       <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1899,7 +3301,7 @@
       <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -1908,7 +3310,7 @@
       <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -1917,16 +3319,16 @@
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -1935,11 +3337,11 @@
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C9" s="10"/>
     </row>
@@ -1947,25 +3349,25 @@
       <c r="A10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>76</v>
+      <c r="A11" s="12"/>
+      <c r="B11" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>46</v>
+      <c r="A12" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>36</v>
@@ -1973,17 +3375,17 @@
       <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>36</v>
@@ -1991,8 +3393,8 @@
       <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>50</v>
+      <c r="A15" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>36</v>
@@ -2001,11 +3403,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -2015,6 +3412,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2024,7 +3426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CDB294D-0E0B-4758-949B-0D567430F7C6}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
@@ -2039,22 +3441,22 @@
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="7"/>
+      <c r="B1" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -2063,7 +3465,7 @@
       <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -2072,7 +3474,7 @@
       <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -2081,7 +3483,7 @@
       <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -2090,29 +3492,29 @@
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C9" s="10"/>
     </row>
@@ -2120,77 +3522,77 @@
       <c r="A10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
-      <c r="B11" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>57</v>
+      <c r="B11" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14" t="s">
-        <v>60</v>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
-      <c r="B13" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>84</v>
+      <c r="B13" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14" t="s">
-        <v>85</v>
+      <c r="A14" s="12"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="14" t="s">
+      <c r="B17" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="10"/>
-    </row>
-    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>36</v>
@@ -2198,8 +3600,8 @@
       <c r="C18" s="10"/>
     </row>
     <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>50</v>
+      <c r="A19" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>36</v>
@@ -2208,11 +3610,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B17:C17"/>
@@ -2222,6 +3619,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2246,22 +3648,22 @@
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="7"/>
+      <c r="B1" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -2270,7 +3672,7 @@
       <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -2279,7 +3681,7 @@
       <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -2288,7 +3690,7 @@
       <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -2297,29 +3699,29 @@
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C9" s="10"/>
     </row>
@@ -2327,70 +3729,70 @@
       <c r="A10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14" t="s">
-        <v>92</v>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
-      <c r="B12" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>94</v>
+      <c r="B12" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>96</v>
+      <c r="A13" s="12"/>
+      <c r="B13" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="14" t="s">
+      <c r="B16" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="10"/>
-    </row>
-    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>36</v>
@@ -2398,8 +3800,8 @@
       <c r="C17" s="10"/>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>50</v>
+      <c r="A18" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>36</v>
@@ -2408,11 +3810,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B16:C16"/>
@@ -2422,6 +3819,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Replaced RecordRTC script src
- Deleted t syllable
- Updated Figures that contain t
- Minor Fixed
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabagita Ivan\Desktop\Skripsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC983136-3BFC-4872-9ADD-03BBD2669C4E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F3AC47-5D5C-45A5-A6AB-68FF4D90649F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{8639E025-6890-4D88-A143-6E789D4DC52A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="13" activeTab="19" xr2:uid="{8639E025-6890-4D88-A143-6E789D4DC52A}"/>
   </bookViews>
   <sheets>
     <sheet name="3.1" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="165">
   <si>
     <t>No</t>
   </si>
@@ -509,9 +509,6 @@
   </si>
   <si>
     <t>i</t>
-  </si>
-  <si>
-    <t>t</t>
   </si>
   <si>
     <t>na</t>
@@ -705,16 +702,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1042,7 +1039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC4C3623-1849-4364-A121-3CC58B3A593B}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1934,10 +1931,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5626A6E2-3CB9-4228-9242-32A8CDB5C5F8}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F14"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2014,7 +2011,7 @@
     </row>
     <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>156</v>
@@ -2028,7 +2025,7 @@
     </row>
     <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>157</v>
@@ -2042,7 +2039,7 @@
     </row>
     <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>158</v>
@@ -2056,7 +2053,7 @@
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>159</v>
@@ -2070,7 +2067,7 @@
     </row>
     <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>160</v>
@@ -2084,7 +2081,7 @@
     </row>
     <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>161</v>
@@ -2098,7 +2095,7 @@
     </row>
     <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>162</v>
@@ -2112,7 +2109,7 @@
     </row>
     <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>163</v>
@@ -2126,7 +2123,7 @@
     </row>
     <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>164</v>
@@ -2135,20 +2132,6 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2159,10 +2142,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D33671-D8B4-4307-A64E-64BE16F5FD15}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F14"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2239,7 +2222,7 @@
     </row>
     <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>156</v>
@@ -2253,7 +2236,7 @@
     </row>
     <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>157</v>
@@ -2267,7 +2250,7 @@
     </row>
     <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>158</v>
@@ -2281,7 +2264,7 @@
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>159</v>
@@ -2295,7 +2278,7 @@
     </row>
     <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>160</v>
@@ -2309,7 +2292,7 @@
     </row>
     <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>161</v>
@@ -2323,7 +2306,7 @@
     </row>
     <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>162</v>
@@ -2337,7 +2320,7 @@
     </row>
     <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>163</v>
@@ -2351,7 +2334,7 @@
     </row>
     <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>164</v>
@@ -2360,20 +2343,6 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2419,10 +2388,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F672DFE2-C1D2-4C9E-9FCE-701CE27F0D30}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2499,7 +2468,7 @@
     </row>
     <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>156</v>
@@ -2513,7 +2482,7 @@
     </row>
     <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>157</v>
@@ -2527,7 +2496,7 @@
     </row>
     <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>158</v>
@@ -2541,7 +2510,7 @@
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>159</v>
@@ -2555,7 +2524,7 @@
     </row>
     <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>160</v>
@@ -2569,7 +2538,7 @@
     </row>
     <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>161</v>
@@ -2583,7 +2552,7 @@
     </row>
     <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>162</v>
@@ -2597,7 +2566,7 @@
     </row>
     <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>163</v>
@@ -2611,7 +2580,7 @@
     </row>
     <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>164</v>
@@ -2620,20 +2589,6 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2721,76 +2676,76 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:3" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -2801,7 +2756,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="8" t="s">
         <v>44</v>
       </c>
@@ -2813,40 +2768,45 @@
       <c r="A12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="10"/>
+      <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="10"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -2856,11 +2816,6 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2894,76 +2849,76 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -2974,7 +2929,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="8" t="s">
         <v>98</v>
       </c>
@@ -2983,7 +2938,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -2994,7 +2949,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="8" t="s">
         <v>54</v>
       </c>
@@ -3006,31 +2961,36 @@
       <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="10"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B14:C14"/>
@@ -3040,11 +3000,6 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3078,76 +3033,76 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -3186,7 +3141,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
         <v>63</v>
@@ -3196,40 +3151,45 @@
       <c r="A16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
@@ -3239,11 +3199,6 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3277,76 +3232,76 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:3" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -3357,7 +3312,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="8" t="s">
         <v>70</v>
       </c>
@@ -3369,40 +3324,45 @@
       <c r="A12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="10"/>
+      <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="10"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -3412,11 +3372,6 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3450,76 +3405,76 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -3555,14 +3510,14 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -3573,7 +3528,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="8" t="s">
         <v>81</v>
       </c>
@@ -3585,31 +3540,36 @@
       <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B17:C17"/>
@@ -3619,11 +3579,6 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3657,76 +3612,76 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -3753,7 +3708,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="8" t="s">
         <v>90</v>
       </c>
@@ -3762,7 +3717,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -3773,7 +3728,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="8" t="s">
         <v>81</v>
       </c>
@@ -3785,31 +3740,36 @@
       <c r="A16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B16:C16"/>
@@ -3819,11 +3779,6 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Tester 1 and 4
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabagita Ivan\Desktop\Skripsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F3AC47-5D5C-45A5-A6AB-68FF4D90649F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B63C94-201A-4DE5-AB15-52D5CFF6AB39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="13" activeTab="19" xr2:uid="{8639E025-6890-4D88-A143-6E789D4DC52A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="16" activeTab="25" xr2:uid="{8639E025-6890-4D88-A143-6E789D4DC52A}"/>
   </bookViews>
   <sheets>
     <sheet name="3.1" sheetId="6" r:id="rId1"/>
@@ -30,9 +30,18 @@
     <sheet name="6.1" sheetId="15" r:id="rId15"/>
     <sheet name="6.2" sheetId="16" r:id="rId16"/>
     <sheet name="6.3" sheetId="17" r:id="rId17"/>
-    <sheet name="6.4" sheetId="18" r:id="rId18"/>
-    <sheet name="6.5" sheetId="19" r:id="rId19"/>
-    <sheet name="6.6" sheetId="20" r:id="rId20"/>
+    <sheet name="6.4" sheetId="21" r:id="rId18"/>
+    <sheet name="6.5" sheetId="22" r:id="rId19"/>
+    <sheet name="6.6" sheetId="23" r:id="rId20"/>
+    <sheet name="6.7" sheetId="24" r:id="rId21"/>
+    <sheet name="6.8" sheetId="25" r:id="rId22"/>
+    <sheet name="6.9" sheetId="26" r:id="rId23"/>
+    <sheet name="6.10" sheetId="27" r:id="rId24"/>
+    <sheet name="6.11" sheetId="28" r:id="rId25"/>
+    <sheet name="6.12" sheetId="29" r:id="rId26"/>
+    <sheet name="6.13" sheetId="30" r:id="rId27"/>
+    <sheet name="6.14" sheetId="31" r:id="rId28"/>
+    <sheet name="6.15" sheetId="32" r:id="rId29"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="186">
   <si>
     <t>No</t>
   </si>
@@ -490,24 +499,15 @@
     <t>Direct back to Home page from Generate page</t>
   </si>
   <si>
-    <t>Syllable</t>
-  </si>
-  <si>
     <t>Noisy Background</t>
   </si>
   <si>
     <t>Semi Noisy Background</t>
   </si>
   <si>
-    <t>No Noisy Background</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
-    <t>/3</t>
-  </si>
-  <si>
     <t>i</t>
   </si>
   <si>
@@ -539,13 +539,133 @@
   </si>
   <si>
     <t>Unknown 3</t>
+  </si>
+  <si>
+    <t>Spoken Syllable</t>
+  </si>
+  <si>
+    <t>Correct Result</t>
+  </si>
+  <si>
+    <t>(a)</t>
+  </si>
+  <si>
+    <t>(unknown)</t>
+  </si>
+  <si>
+    <t>(na)</t>
+  </si>
+  <si>
+    <t>(ri)</t>
+  </si>
+  <si>
+    <t>(ma)</t>
+  </si>
+  <si>
+    <t>0/3</t>
+  </si>
+  <si>
+    <t>(kan)</t>
+  </si>
+  <si>
+    <t>(ku)</t>
+  </si>
+  <si>
+    <t>(mu)</t>
+  </si>
+  <si>
+    <t>(o)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Unknown 3 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(mi)</t>
+    </r>
+  </si>
+  <si>
+    <t>1/3</t>
+  </si>
+  <si>
+    <t>3/3</t>
+  </si>
+  <si>
+    <t>2/3</t>
+  </si>
+  <si>
+    <t>(silent)</t>
+  </si>
+  <si>
+    <t>(mi)</t>
+  </si>
+  <si>
+    <t>(i)</t>
+  </si>
+  <si>
+    <t>(di)</t>
+  </si>
+  <si>
+    <t>Not Noisy Background</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">40 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(unknown)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">60 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(unknown)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">100 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(unknown)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -566,6 +686,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -575,7 +702,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -672,11 +799,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -702,16 +860,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -722,6 +880,48 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1930,423 +2130,1012 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5626A6E2-3CB9-4228-9242-32A8CDB5C5F8}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB235EE6-0BED-45E7-9E95-2AAA9EE97E66}">
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16">
+        <v>2</v>
+      </c>
+      <c r="E2" s="16">
+        <v>3</v>
+      </c>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="C3" s="17">
+        <v>52</v>
+      </c>
+      <c r="D3" s="17">
+        <v>100</v>
+      </c>
+      <c r="E3" s="17">
+        <v>100</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" s="28"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>2</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="C5" s="17">
+        <v>62</v>
+      </c>
+      <c r="D5" s="17">
+        <v>85</v>
+      </c>
+      <c r="E5" s="17">
+        <v>96</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F6" s="25"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>3</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="C7" s="17">
+        <v>100</v>
+      </c>
+      <c r="D7" s="17">
+        <v>86</v>
+      </c>
+      <c r="E7" s="17">
+        <v>100</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F8" s="25"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>4</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="C9" s="17">
+        <v>100</v>
+      </c>
+      <c r="D9" s="17">
+        <v>84</v>
+      </c>
+      <c r="E9" s="17">
+        <v>100</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>5</v>
+      </c>
+      <c r="B11" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="C11" s="17">
+        <v>99</v>
+      </c>
+      <c r="D11" s="17">
+        <v>71</v>
+      </c>
+      <c r="E11" s="17">
+        <v>88</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" s="25"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>6</v>
+      </c>
+      <c r="B13" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="C13" s="17">
+        <v>59</v>
+      </c>
+      <c r="D13" s="17">
+        <v>100</v>
+      </c>
+      <c r="E13" s="17">
+        <v>97</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F14" s="25"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>7</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="C15" s="26">
+        <v>50</v>
+      </c>
+      <c r="D15" s="26">
+        <v>100</v>
+      </c>
+      <c r="E15" s="26">
+        <v>92</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="F16" s="28"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>8</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="C17" s="17">
+        <v>100</v>
+      </c>
+      <c r="D17" s="17">
+        <v>85</v>
+      </c>
+      <c r="E17" s="17">
+        <v>100</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="F18" s="28"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>9</v>
+      </c>
+      <c r="B19" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="C19" s="17">
+        <v>72</v>
+      </c>
+      <c r="D19" s="17">
+        <v>61</v>
+      </c>
+      <c r="E19" s="17">
+        <v>79</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="F20" s="28"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>10</v>
+      </c>
+      <c r="B21" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="C21" s="26">
+        <v>99</v>
+      </c>
+      <c r="D21" s="26">
+        <v>100</v>
+      </c>
+      <c r="E21" s="26">
+        <v>99</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25"/>
+      <c r="B22" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>11</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="C23" s="17">
+        <v>100</v>
+      </c>
+      <c r="D23" s="17">
+        <v>100</v>
+      </c>
+      <c r="E23" s="17">
+        <v>100</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25"/>
+      <c r="B24" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="F24" s="25"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>12</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="C25" s="17">
+        <v>100</v>
+      </c>
+      <c r="D25" s="17">
+        <v>51</v>
+      </c>
+      <c r="E25" s="17">
+        <v>96</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25"/>
+      <c r="B26" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
-        <v>153</v>
-      </c>
+      <c r="D26" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F26" s="28"/>
     </row>
   </sheetData>
+  <mergeCells count="37">
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="F3:F4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D33671-D8B4-4307-A64E-64BE16F5FD15}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990F6455-69A2-4ED3-AA4B-531CC03D46B0}">
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16">
+        <v>2</v>
+      </c>
+      <c r="E2" s="16">
+        <v>3</v>
+      </c>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="C3" s="17">
+        <v>100</v>
+      </c>
+      <c r="D3" s="17">
+        <v>100</v>
+      </c>
+      <c r="E3" s="17">
+        <v>100</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="F4" s="28"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>2</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="C5" s="17">
+        <v>100</v>
+      </c>
+      <c r="D5" s="17">
+        <v>36</v>
+      </c>
+      <c r="E5" s="17">
+        <v>100</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="28"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>3</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="C7" s="17">
+        <v>97</v>
+      </c>
+      <c r="D7" s="17">
+        <v>48</v>
+      </c>
+      <c r="E7" s="17">
+        <v>99</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" s="28"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>4</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="C9" s="17">
+        <v>49</v>
+      </c>
+      <c r="D9" s="17">
+        <v>98</v>
+      </c>
+      <c r="E9" s="17">
+        <v>79</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>5</v>
+      </c>
+      <c r="B11" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="C11" s="17">
+        <v>55</v>
+      </c>
+      <c r="D11" s="17">
+        <v>99</v>
+      </c>
+      <c r="E11" s="17">
+        <v>50</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F12" s="25"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>6</v>
+      </c>
+      <c r="B13" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="C13" s="17">
+        <v>57</v>
+      </c>
+      <c r="D13" s="17">
+        <v>100</v>
+      </c>
+      <c r="E13" s="17">
+        <v>100</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="F14" s="28"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>7</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="C15" s="17">
+        <v>100</v>
+      </c>
+      <c r="D15" s="17">
+        <v>75</v>
+      </c>
+      <c r="E15" s="17">
+        <v>100</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F16" s="28"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>8</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="C17" s="17">
+        <v>92</v>
+      </c>
+      <c r="D17" s="17">
+        <v>68</v>
+      </c>
+      <c r="E17" s="17">
+        <v>91</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="F18" s="28"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>9</v>
+      </c>
+      <c r="B19" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="C19" s="17">
+        <v>100</v>
+      </c>
+      <c r="D19" s="17">
+        <v>94</v>
+      </c>
+      <c r="E19" s="17">
+        <v>100</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="F20" s="28"/>
+    </row>
+    <row r="21" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>10</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="C21" s="17">
+        <v>100</v>
+      </c>
+      <c r="D21" s="17">
+        <v>99</v>
+      </c>
+      <c r="E21" s="17">
+        <v>100</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25"/>
+      <c r="B22" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>11</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="C23" s="17">
+        <v>100</v>
+      </c>
+      <c r="D23" s="17">
+        <v>89</v>
+      </c>
+      <c r="E23" s="17">
+        <v>72</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25"/>
+      <c r="B24" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="F24" s="28"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>12</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
-        <v>153</v>
-      </c>
+      <c r="C25" s="17">
+        <v>100</v>
+      </c>
+      <c r="D25" s="17">
+        <v>94</v>
+      </c>
+      <c r="E25" s="17">
+        <v>100</v>
+      </c>
+      <c r="F25" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25"/>
+      <c r="B26" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F26" s="25"/>
     </row>
   </sheetData>
+  <mergeCells count="37">
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="F3:F4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2387,212 +3176,2084 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F672DFE2-C1D2-4C9E-9FCE-701CE27F0D30}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FAAF9FA-F3D9-4C22-BE64-9E20341CE5D8}">
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16">
+        <v>2</v>
+      </c>
+      <c r="E2" s="16">
+        <v>3</v>
+      </c>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="17">
+        <v>100</v>
+      </c>
+      <c r="D3" s="17">
+        <v>100</v>
+      </c>
+      <c r="E3" s="17">
+        <v>100</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="F4" s="28"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>2</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="17">
+        <v>94</v>
+      </c>
+      <c r="D5" s="17">
+        <v>48</v>
+      </c>
+      <c r="E5" s="17">
+        <v>94</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="28"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>3</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="17">
+        <v>80</v>
+      </c>
+      <c r="D7" s="17">
+        <v>99</v>
+      </c>
+      <c r="E7" s="17">
+        <v>100</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" s="28"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>4</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="17">
+        <v>96</v>
+      </c>
+      <c r="D9" s="17">
+        <v>90</v>
+      </c>
+      <c r="E9" s="17">
+        <v>57</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>5</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="17">
+        <v>100</v>
+      </c>
+      <c r="D11" s="17">
+        <v>86</v>
+      </c>
+      <c r="E11" s="17">
+        <v>95</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="F12" s="25"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>6</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="17">
+        <v>99</v>
+      </c>
+      <c r="D13" s="17">
+        <v>100</v>
+      </c>
+      <c r="E13" s="17">
+        <v>80</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F14" s="25"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>7</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="17">
+        <v>100</v>
+      </c>
+      <c r="D15" s="17">
+        <v>96</v>
+      </c>
+      <c r="E15" s="17">
+        <v>91</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F16" s="28"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>8</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="17">
+        <v>85</v>
+      </c>
+      <c r="D17" s="17">
+        <v>96</v>
+      </c>
+      <c r="E17" s="17">
+        <v>100</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="F18" s="28"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>9</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" s="17">
+        <v>92</v>
+      </c>
+      <c r="D19" s="17">
+        <v>100</v>
+      </c>
+      <c r="E19" s="17">
+        <v>100</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="F20" s="28"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>10</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" s="26">
+        <v>98</v>
+      </c>
+      <c r="D21" s="26">
+        <v>98</v>
+      </c>
+      <c r="E21" s="26">
+        <v>98</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25"/>
+      <c r="B22" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>11</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" s="17">
+        <v>100</v>
+      </c>
+      <c r="D23" s="17">
+        <v>98</v>
+      </c>
+      <c r="E23" s="17">
+        <v>65</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25"/>
+      <c r="B24" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="F24" s="28"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>12</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" s="17">
+        <v>54</v>
+      </c>
+      <c r="D25" s="17">
+        <v>100</v>
+      </c>
+      <c r="E25" s="17">
+        <v>67</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25"/>
+      <c r="B26" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="F26" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="37">
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="F3:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2D21D3-314A-4749-8C34-D06786D3AE8C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F04D4AB-F3EF-43C2-BE11-8B76C72C9550}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE69C378-7CEF-4D0C-943B-C5293127ACA7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB9F02B-1A08-466C-8127-2C1E153A2A6A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A17526-1A85-46EF-B7A0-CEFEEDB9C956}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95FED96E-7886-433A-9289-8A2020F935CB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H13:H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04000B9-11A2-439A-84D6-38C2103A3796}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="A1:F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16">
+        <v>2</v>
+      </c>
+      <c r="E2" s="16">
+        <v>3</v>
+      </c>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="17">
+        <v>100</v>
+      </c>
+      <c r="D3" s="17">
+        <v>99</v>
+      </c>
+      <c r="E3" s="17">
+        <v>94</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4" s="25"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>2</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="17">
+        <v>97</v>
+      </c>
+      <c r="D5" s="17">
+        <v>99</v>
+      </c>
+      <c r="E5" s="17">
+        <v>99</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" s="25"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>3</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="17">
+        <v>100</v>
+      </c>
+      <c r="D7" s="17">
+        <v>99</v>
+      </c>
+      <c r="E7" s="17">
+        <v>99</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" s="28"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>4</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="17">
+        <v>93</v>
+      </c>
+      <c r="D9" s="17">
+        <v>99</v>
+      </c>
+      <c r="E9" s="17">
+        <v>100</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" s="28"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>5</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="17">
+        <v>55</v>
+      </c>
+      <c r="D11" s="17">
+        <v>99</v>
+      </c>
+      <c r="E11" s="17">
+        <v>43</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" s="25"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>6</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="17">
+        <v>99</v>
+      </c>
+      <c r="D13" s="17">
+        <v>54</v>
+      </c>
+      <c r="E13" s="17">
+        <v>99</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F14" s="25"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>7</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="17">
+        <v>97</v>
+      </c>
+      <c r="D15" s="17">
+        <v>74</v>
+      </c>
+      <c r="E15" s="17">
+        <v>100</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F16" s="28"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>8</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="17">
+        <v>68</v>
+      </c>
+      <c r="D17" s="17">
+        <v>92</v>
+      </c>
+      <c r="E17" s="17">
+        <v>52</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="E18" s="18">
+        <v>-52</v>
+      </c>
+      <c r="F18" s="28"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>9</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" s="17">
+        <v>48</v>
+      </c>
+      <c r="D19" s="17">
+        <v>22</v>
+      </c>
+      <c r="E19" s="17">
+        <v>99</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="F20" s="25"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>10</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="D21" s="17">
+        <v>100</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25"/>
+      <c r="B22" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="25"/>
+      <c r="D22" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" s="25"/>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>11</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" s="17">
+        <v>100</v>
+      </c>
+      <c r="D23" s="17">
+        <v>100</v>
+      </c>
+      <c r="E23" s="17">
+        <v>100</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25"/>
+      <c r="B24" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="F24" s="25"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>12</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25" s="17">
+        <v>55</v>
+      </c>
+      <c r="D25" s="17">
+        <v>99</v>
+      </c>
+      <c r="E25" s="17">
+        <v>94</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="F26" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="40">
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="F3:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A73946DF-36BA-430D-9B02-A367DD4E7DD9}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16">
+        <v>2</v>
+      </c>
+      <c r="E2" s="16">
+        <v>3</v>
+      </c>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="C3" s="17">
+        <v>73</v>
+      </c>
+      <c r="D3" s="17">
+        <v>91</v>
+      </c>
+      <c r="E3" s="17">
+        <v>99</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" s="25"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>2</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>101</v>
+      <c r="C5" s="17">
+        <v>81</v>
+      </c>
+      <c r="D5" s="17">
+        <v>99</v>
+      </c>
+      <c r="E5" s="17">
+        <v>100</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" s="28"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>3</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="17">
+        <v>100</v>
+      </c>
+      <c r="D7" s="17">
+        <v>99</v>
+      </c>
+      <c r="E7" s="17">
+        <v>99</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F8" s="25"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>4</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="17">
+        <v>99</v>
+      </c>
+      <c r="D9" s="17">
+        <v>99</v>
+      </c>
+      <c r="E9" s="17">
+        <v>78</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F10" s="28"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>5</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="17">
+        <v>81</v>
+      </c>
+      <c r="D11" s="17">
+        <v>99</v>
+      </c>
+      <c r="E11" s="17">
+        <v>99</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" s="25"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>6</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="17">
+        <v>100</v>
+      </c>
+      <c r="D13" s="17">
+        <v>99</v>
+      </c>
+      <c r="E13" s="17">
+        <v>99</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="F14" s="25"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>7</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="17">
+        <v>85</v>
+      </c>
+      <c r="D15" s="17">
+        <v>99</v>
+      </c>
+      <c r="E15" s="17">
+        <v>98</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F16" s="28"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>8</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="17">
+        <v>96</v>
+      </c>
+      <c r="D17" s="17">
+        <v>89</v>
+      </c>
+      <c r="E17" s="17">
+        <v>99</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="F18" s="28"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>9</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" s="17">
+        <v>100</v>
+      </c>
+      <c r="D19" s="17">
+        <v>99</v>
+      </c>
+      <c r="E19" s="17">
+        <v>64</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F20" s="25"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>10</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" s="26">
+        <v>99</v>
+      </c>
+      <c r="D21" s="26">
+        <v>99</v>
+      </c>
+      <c r="E21" s="26">
+        <v>100</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25"/>
+      <c r="B22" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>11</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" s="17">
+        <v>99</v>
+      </c>
+      <c r="D23" s="17">
+        <v>100</v>
+      </c>
+      <c r="E23" s="17">
+        <v>99</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25"/>
+      <c r="B24" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="F24" s="25"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>12</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25" s="17">
+        <v>43</v>
+      </c>
+      <c r="D25" s="17">
+        <v>59</v>
+      </c>
+      <c r="E25" s="17">
+        <v>99</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F26" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="38">
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="F3:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7118C7DD-D063-4FB7-8E1E-913536BEA5FB}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21:F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="19" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="16">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="16">
+        <v>2</v>
+      </c>
+      <c r="E2" s="16">
+        <v>3</v>
+      </c>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="17">
+        <v>99</v>
+      </c>
+      <c r="D3" s="17">
+        <v>75</v>
+      </c>
+      <c r="E3" s="17">
+        <v>100</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="F4" s="28"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>2</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="17">
+        <v>88</v>
+      </c>
+      <c r="D5" s="17">
+        <v>99</v>
+      </c>
+      <c r="E5" s="17">
+        <v>99</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" s="28"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>3</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="C7" s="17">
+        <v>99</v>
+      </c>
+      <c r="D7" s="17">
+        <v>99</v>
+      </c>
+      <c r="E7" s="17">
+        <v>99</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" s="28"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>4</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="C9" s="17">
+        <v>55</v>
+      </c>
+      <c r="D9" s="17">
+        <v>72</v>
+      </c>
+      <c r="E9" s="17">
+        <v>99</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>5</v>
+      </c>
+      <c r="B11" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="C11" s="17">
+        <v>99</v>
+      </c>
+      <c r="D11" s="17">
+        <v>94</v>
+      </c>
+      <c r="E11" s="17">
+        <v>28</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="F12" s="25"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>6</v>
+      </c>
+      <c r="B13" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="C13" s="17">
+        <v>89</v>
+      </c>
+      <c r="D13" s="17">
+        <v>99</v>
+      </c>
+      <c r="E13" s="17">
+        <v>99</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F14" s="25"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>7</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="C15" s="17">
+        <v>99</v>
+      </c>
+      <c r="D15" s="17">
+        <v>100</v>
+      </c>
+      <c r="E15" s="17">
+        <v>99</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F16" s="28"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>8</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="C17" s="17">
+        <v>39</v>
+      </c>
+      <c r="D17" s="17">
+        <v>99</v>
+      </c>
+      <c r="E17" s="17">
+        <v>58</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="F18" s="28"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>9</v>
+      </c>
+      <c r="B19" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="C19" s="17">
+        <v>100</v>
+      </c>
+      <c r="D19" s="17">
+        <v>99</v>
+      </c>
+      <c r="E19" s="17">
+        <v>100</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="F20" s="28"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>10</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="C21" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="D21" s="17">
+        <v>24</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25"/>
+      <c r="B22" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="25"/>
+      <c r="D22" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" s="25"/>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>11</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="C23" s="17">
+        <v>100</v>
+      </c>
+      <c r="D23" s="17">
+        <v>99</v>
+      </c>
+      <c r="E23" s="17">
+        <v>100</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25"/>
+      <c r="B24" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="F24" s="25"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
-        <v>153</v>
-      </c>
+      <c r="B25" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25" s="17">
+        <v>60</v>
+      </c>
+      <c r="D25" s="17">
+        <v>100</v>
+      </c>
+      <c r="E25" s="17">
+        <v>99</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F26" s="28"/>
     </row>
   </sheetData>
+  <mergeCells count="40">
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="F3:F4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2676,76 +5337,76 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -2756,7 +5417,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="8" t="s">
         <v>44</v>
       </c>
@@ -2768,45 +5429,40 @@
       <c r="A12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -2816,6 +5472,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2849,76 +5510,76 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -2929,7 +5590,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="8" t="s">
         <v>98</v>
       </c>
@@ -2938,7 +5599,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -2949,7 +5610,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>54</v>
       </c>
@@ -2961,36 +5622,31 @@
       <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="10"/>
     </row>
     <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B14:C14"/>
@@ -3000,6 +5656,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3033,76 +5694,76 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -3141,7 +5802,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
         <v>63</v>
@@ -3151,45 +5812,40 @@
       <c r="A16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="10"/>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="10"/>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
@@ -3199,6 +5855,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3232,76 +5893,76 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -3312,7 +5973,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="8" t="s">
         <v>70</v>
       </c>
@@ -3324,45 +5985,40 @@
       <c r="A12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -3372,6 +6028,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3405,76 +6066,76 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -3510,14 +6171,14 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -3528,7 +6189,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="8" t="s">
         <v>81</v>
       </c>
@@ -3540,36 +6201,31 @@
       <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="10"/>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B17:C17"/>
@@ -3579,6 +6235,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3612,76 +6273,76 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -3708,7 +6369,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>90</v>
       </c>
@@ -3717,7 +6378,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -3728,7 +6389,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="8" t="s">
         <v>81</v>
       </c>
@@ -3740,36 +6401,31 @@
       <c r="A16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="10"/>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="10"/>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B16:C16"/>
@@ -3779,6 +6435,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>